<commit_message>
add & modify data
</commit_message>
<xml_diff>
--- a/xgbXXI.xlsx
+++ b/xgbXXI.xlsx
@@ -16,19 +16,21 @@
     <sheet name="pr.rdf.III" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">mdaIII!$B$1:$B$9</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'pr.I'!$A$1:$A$17</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'clu.xgbXXI'!$B$1:$B$8</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">mdaIII!$B$1:$B$17</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'pr.I'!$A$1:$A$25</definedName>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'pr.rdf.III'!$A$1:$A$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'pr.XXI'!$A$1:$A$17</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">xgbXXI!$B$1:$B$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'pr.XXI'!$A$1:$A$25</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">xgbXXI!$B$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">xgbXXI!$B$1:$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">xgbXXI!$B$1:$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">xgbXXI!$B$1:$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0" vbProcedure="false">xgbXXI!$B$1:$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">xgbXXI!$B$1:$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">xgbXXI!$B$1:$B$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">xgbXXI!$B$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">xgbXXI!$B$1:$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">xgbXXI!$B$1:$B$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">xgbXXI!$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">xgbXXI!$B$1:$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">mdaIII!$B$1:$B$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0" vbProcedure="false">mdaIII!$B$1:$B$6</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0" vbProcedure="false">mdaIII!$B$1:$B$5</definedName>
@@ -36,6 +38,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">mdaIII!$B$1:$B$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">mdaIII!$B$1:$B$9</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">mdaIII!$B$1:$B$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">mdaIII!$B$1:$B$9</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">'pr.I'!$A$1:$A$15</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">'pr.I'!$A$1:$A$15</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">'pr.I'!$A$1:$A$11</definedName>
@@ -48,6 +51,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'pr.I'!$A$2:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'pr.I'!$A$1:$A$17</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'pr.I'!$A$1:$A$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'pr.I'!$A$1:$A$17</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'pr.XXI'!$A$1:$A$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'pr.XXI'!$A$1:$A$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'pr.XXI'!$A$1:$A$11</definedName>
@@ -60,8 +64,10 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'pr.XXI'!$A$2:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'pr.XXI'!$A$1:$A$17</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'pr.XXI'!$A$1:$A$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'pr.XXI'!$A$1:$A$17</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'pr.rdf.III'!$A$1:$A$3</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'pr.rdf.III'!$A$1:$A$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'pr.rdf.III'!$A$1:$A$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -73,12 +79,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t xml:space="preserve">15\14</t>
   </si>
   <si>
     <t xml:space="preserve">9\10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6\5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14\13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15\16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19\20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25\26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4\3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30\29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5\4</t>
   </si>
   <si>
     <t xml:space="preserve">22\23</t>
@@ -99,9 +129,6 @@
     <t xml:space="preserve">9\8</t>
   </si>
   <si>
-    <t xml:space="preserve">25\26</t>
-  </si>
-  <si>
     <t xml:space="preserve">33\34</t>
   </si>
   <si>
@@ -114,13 +141,7 @@
     <t xml:space="preserve">24\26</t>
   </si>
   <si>
-    <t xml:space="preserve">6\5</t>
-  </si>
-  <si>
     <t xml:space="preserve">6\7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4\3</t>
   </si>
   <si>
     <t xml:space="preserve">10\11</t>
@@ -137,6 +158,15 @@
   <si>
     <t xml:space="preserve">5\6</t>
   </si>
+  <si>
+    <t xml:space="preserve">14\15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29\30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26\25</t>
+  </si>
 </sst>
 </file>
 
@@ -146,7 +176,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -184,6 +214,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFFF6600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF3333FF"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -205,7 +242,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF6600"/>
+      <color rgb="FFFF9900"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -279,7 +316,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -296,10 +333,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -308,11 +341,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -328,19 +365,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,6 +477,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -448,24 +493,22 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="2.29591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="2.15816326530612"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="3" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="6.01020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="3" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="6.01020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="5.80612244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="3" width="6.01020408163265"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="3" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="3" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="3" width="7.1530612244898"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1" s="4"/>
-    </row>
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>2018096</v>
@@ -473,10 +516,10 @@
       <c r="B2" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="D2" s="6" t="n">
+      <c r="C2" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="n">
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -502,7 +545,7 @@
       <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="4" t="n">
         <v>8</v>
       </c>
       <c r="D3" s="3" t="n">
@@ -520,8 +563,153 @@
       <c r="H3" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>1</v>
+      <c r="I3" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2018098</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2018099</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>2018100</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>2018101</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>2018102</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -539,7 +727,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="B1:B2"/>
+  <autoFilter ref="B1:B8"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -556,27 +744,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="2.29591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="2.15816326530612"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.01020408163265"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="3.78061224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="6.01020408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="3.64285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,14 +778,14 @@
       <c r="B2" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="4" t="n">
         <v>21</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>29</v>
@@ -619,26 +807,26 @@
       <c r="B3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="4" t="n">
         <v>3</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,7 +836,7 @@
       <c r="B4" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="4" t="n">
         <v>8</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -658,10 +846,10 @@
         <v>21</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>1</v>
@@ -677,7 +865,7 @@
       <c r="B5" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="4" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -687,7 +875,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>30</v>
@@ -710,10 +898,10 @@
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F6" s="9" t="n">
         <v>31</v>
@@ -735,11 +923,11 @@
       <c r="B7" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E7" s="9" t="n">
         <v>14</v>
@@ -764,7 +952,7 @@
       <c r="B8" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="4" t="n">
         <v>5</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -774,16 +962,16 @@
         <v>14</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G8" s="9" t="n">
         <v>33</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,11 +981,11 @@
       <c r="B9" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="4" t="n">
         <v>3</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E9" s="9" t="n">
         <v>16</v>
@@ -806,13 +994,13 @@
         <v>18</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,19 +1011,19 @@
         <v>3</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>25</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>2</v>
@@ -851,7 +1039,7 @@
       <c r="B11" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="11" t="n">
@@ -864,10 +1052,10 @@
         <v>24</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>12</v>
@@ -880,13 +1068,13 @@
       <c r="B12" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="0" t="n">
+      <c r="C12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="11" t="n">
         <v>18</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -899,11 +1087,156 @@
         <v>10</v>
       </c>
       <c r="I12" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
+        <v>2018098</v>
+      </c>
+      <c r="B13" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <v>27</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
+        <v>2018099</v>
+      </c>
+      <c r="B14" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" s="11" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="n">
+        <v>2018100</v>
+      </c>
+      <c r="B15" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F15" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="n">
+        <v>2018101</v>
+      </c>
+      <c r="B16" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="n">
+        <v>2018102</v>
+      </c>
+      <c r="B17" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="G17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B9"/>
+  <autoFilter ref="B1:B17"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -920,29 +1253,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="2.29591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="2.15816326530612"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="3" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="3" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="6.01020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="4.72448979591837"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="3" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="3" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="3" width="7.1530612244898"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1" s="4"/>
-    </row>
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>2018096</v>
@@ -950,13 +1283,13 @@
       <c r="B2" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="4" t="n">
         <v>4</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="5" t="n">
         <v>13</v>
       </c>
       <c r="F2" s="3" t="n">
@@ -968,7 +1301,7 @@
       <c r="H2" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="5" t="n">
         <v>10</v>
       </c>
     </row>
@@ -979,13 +1312,13 @@
       <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="4" t="n">
         <v>8</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="5" t="n">
         <v>18</v>
       </c>
       <c r="F3" s="3" t="n">
@@ -1001,7 +1334,153 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2018098</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2018099</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>2018100</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>2018101</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>2018102</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="B1:B8"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1009,6 +1488,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1017,22 +1497,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="2.29591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="2.15816326530612"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.10714285714286"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.10714285714286"/>
     <col collapsed="false" hidden="false" max="8" min="5" style="0" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,8 +1921,120 @@
         <v>-10</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>-3</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>-3</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>-7</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>-6</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>-6</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>-6</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>-6</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>-6</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>-14</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>-9</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>-5</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>-8</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A17"/>
+  <autoFilter ref="A1:A25"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1460,27 +2051,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A2:I25"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K45" activeCellId="0" sqref="K45"/>
+      <selection pane="bottomLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="2.29591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="2.15816326530612"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="3" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="3" width="3.10714285714286"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="3" width="3.51020408163265"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="3" width="3.10714285714286"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="3" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="3" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="3" width="7.02040816326531"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="n">
         <v>6</v>
       </c>
@@ -1504,7 +2094,7 @@
       </c>
       <c r="H2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="n">
         <v>1</v>
       </c>
@@ -1530,7 +2120,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="n">
         <v>3</v>
       </c>
@@ -1554,7 +2144,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="n">
         <v>6</v>
       </c>
@@ -1578,7 +2168,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="n">
         <v>1</v>
       </c>
@@ -1596,7 +2186,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="n">
         <v>3</v>
       </c>
@@ -1620,7 +2210,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="n">
         <v>6</v>
       </c>
@@ -1644,7 +2234,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
         <v>1</v>
       </c>
@@ -1670,7 +2260,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="n">
         <v>3</v>
       </c>
@@ -1690,7 +2280,7 @@
       </c>
       <c r="H10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="n">
         <v>6</v>
       </c>
@@ -1712,7 +2302,7 @@
       </c>
       <c r="H11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="n">
         <v>1</v>
       </c>
@@ -1738,7 +2328,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="n">
         <v>3</v>
       </c>
@@ -1758,7 +2348,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="n">
         <v>6</v>
       </c>
@@ -1780,7 +2370,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="n">
         <v>1</v>
       </c>
@@ -1800,7 +2390,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="n">
         <v>3</v>
       </c>
@@ -1824,7 +2414,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="n">
         <v>6</v>
       </c>
@@ -1850,7 +2440,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="n">
         <v>1</v>
       </c>
@@ -1872,7 +2462,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="n">
         <v>3</v>
       </c>
@@ -1898,7 +2488,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="n">
         <v>6</v>
       </c>
@@ -1921,8 +2511,121 @@
         <v>-6</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>-2</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>-6</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>-4</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>-4</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>-7</v>
+      </c>
+      <c r="I24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>-5</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>-4</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>-8</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A17"/>
+  <autoFilter ref="A1:A25"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1939,20 +2642,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="2.53571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,25 +2665,25 @@
       <c r="A2" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="4" t="n">
         <v>0.065</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0.032</v>
       </c>
-      <c r="D2" s="14" t="n">
+      <c r="D2" s="15" t="n">
         <v>0.0725</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="4" t="n">
         <v>0.078</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>0.1265</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="H2" s="4" t="n">
         <v>0.0755</v>
       </c>
     </row>
@@ -1988,13 +2691,13 @@
       <c r="A3" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="4" t="n">
         <v>0.105</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.071</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="4" t="n">
         <v>0.105</v>
       </c>
       <c r="E3" s="0" t="n">
@@ -2014,25 +2717,25 @@
       <c r="A4" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="n">
+      <c r="B4" s="16" t="n">
         <v>0.0155</v>
       </c>
-      <c r="C4" s="15" t="n">
+      <c r="C4" s="16" t="n">
         <v>0.0535</v>
       </c>
-      <c r="D4" s="15" t="n">
+      <c r="D4" s="16" t="n">
         <v>0.017</v>
       </c>
-      <c r="E4" s="15" t="n">
+      <c r="E4" s="16" t="n">
         <v>0.098</v>
       </c>
-      <c r="F4" s="15" t="n">
+      <c r="F4" s="16" t="n">
         <v>0.1395</v>
       </c>
-      <c r="G4" s="15" t="n">
+      <c r="G4" s="16" t="n">
         <v>0.0805</v>
       </c>
-      <c r="H4" s="15" t="n">
+      <c r="H4" s="16" t="n">
         <v>0.103</v>
       </c>
     </row>
@@ -2040,25 +2743,25 @@
       <c r="A5" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="4" t="n">
         <v>0.077</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="4" t="n">
         <v>0.046</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="4" t="n">
         <v>0.059</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="4" t="n">
         <v>0.0585</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="4" t="n">
         <v>0.2035</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="4" t="n">
         <v>0.093</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="4" t="n">
         <v>0.2155</v>
       </c>
     </row>
@@ -2066,26 +2769,156 @@
       <c r="A6" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="4" t="n">
         <v>0.0315</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="4" t="n">
         <v>0.074</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="4" t="n">
         <v>0.0415</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="4" t="n">
         <v>0.0405</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="4" t="n">
         <v>0.131</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="4" t="n">
         <v>0.11</v>
       </c>
-      <c r="H6" s="5" t="n">
+      <c r="H6" s="4" t="n">
         <v>0.054</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>0.0195</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>0.215</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.0725</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.1035</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.0955</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.0245</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0.1175</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.131</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.0205</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>0.0225</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>0.0395</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>0.0825</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.1105</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.0205</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.1045</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.0695</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0.0635</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.0595</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.1255</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.0585</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.0485</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.152</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>